<commit_message>
edited dataprovider code and added cucumberrunner xml
</commit_message>
<xml_diff>
--- a/testdata/JustDial_TestData.xlsx
+++ b/testdata/JustDial_TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408440\CTS_TRAINING\Practicals\IntellijSeleniumPracticals\JustDialAutomationMain\JustDialAutomation\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408456\Desktop\CTS_Java_Training\Practicals\SeleniumProjects\JustDialAutomation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E8234F-96AB-414F-9EEC-9728BD08B81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BF3F90-4D63-4CFC-9ED7-5D43CA754E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DE57E9C9-A6C1-4A7D-85B9-1309751074B4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="68">
   <si>
     <t>TC_ID</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -630,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDE3050-D1DC-49F4-900E-5DA4D3857D18}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1011,7 +1014,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
         <v>44</v>
       </c>
@@ -1031,7 +1034,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
         <v>44</v>
       </c>
@@ -1051,7 +1054,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
         <v>45</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
         <v>45</v>
       </c>
@@ -1091,7 +1094,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
added Smoke and Regression Suite
</commit_message>
<xml_diff>
--- a/testdata/JustDial_TestData.xlsx
+++ b/testdata/JustDial_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408456\Desktop\CTS_Java_Training\Practicals\SeleniumProjects\JustDialAutomation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BF3F90-4D63-4CFC-9ED7-5D43CA754E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469030BD-329A-4132-A499-EC425470A9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DE57E9C9-A6C1-4A7D-85B9-1309751074B4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="67">
   <si>
     <t>TC_ID</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Test Data3</t>
   </si>
   <si>
-    <t>Automation Test Script ID</t>
-  </si>
-  <si>
     <t>validateHomePageTitle</t>
   </si>
   <si>
@@ -239,7 +236,7 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>Test Scenario ID</t>
   </si>
 </sst>
 </file>
@@ -633,25 +630,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDE3050-D1DC-49F4-900E-5DA4D3857D18}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="C4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" customWidth="true" width="17.453125"/>
     <col min="3" max="3" customWidth="true" width="42.6328125"/>
     <col min="4" max="4" customWidth="true" width="13.1796875"/>
     <col min="5" max="5" customWidth="true" width="62.453125"/>
     <col min="6" max="6" customWidth="true" width="54.1796875"/>
     <col min="7" max="7" customWidth="true" width="65.7265625"/>
     <col min="8" max="8" customWidth="true" width="19.6328125"/>
-    <col min="9" max="9" customWidth="true" width="10.26953125"/>
-    <col min="10" max="10" customWidth="true" width="11.08984375"/>
+    <col min="9" max="9" customWidth="true" width="11.08984375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -672,446 +669,446 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>9</v>
-      </c>
       <c r="H2" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="H3" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="H4" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>4</v>
       </c>
       <c r="E5" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>40</v>
-      </c>
       <c r="H5" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>4</v>
       </c>
       <c r="E6" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="F6" t="s" s="0">
-        <v>40</v>
-      </c>
       <c r="H6" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s" s="0">
         <v>4</v>
       </c>
       <c r="E7" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="F7" t="s" s="0">
-        <v>40</v>
-      </c>
       <c r="H7" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s" s="0">
         <v>4</v>
       </c>
       <c r="E8" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="F8" t="s" s="0">
-        <v>40</v>
-      </c>
       <c r="H8" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="F9" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="H9" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="F10" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H10" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s" s="0">
         <v>4</v>
       </c>
       <c r="E11" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="F11" t="s" s="0">
-        <v>40</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s" s="0">
         <v>4</v>
       </c>
       <c r="E12" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="F12" t="s" s="0">
-        <v>40</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H12" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="D13" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E13" t="s" s="0">
-        <v>25</v>
-      </c>
       <c r="H13" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s" s="0">
         <v>4</v>
       </c>
       <c r="H14" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s" s="0">
         <v>4</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s" s="0">
         <v>4</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H16" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s" s="0">
         <v>4</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H17" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s" s="0">
         <v>4</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s" s="0">
         <v>4</v>
       </c>
       <c r="H19" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F20" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="D20" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E20" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="F20" t="s" s="0">
-        <v>36</v>
-      </c>
       <c r="H20" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D21" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E21" t="s" s="0">
-        <v>39</v>
-      </c>
       <c r="H21" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>